<commit_message>
route nixie daughter boards
</commit_message>
<xml_diff>
--- a/hardware/BOM-nixieAccurateClock.xlsx
+++ b/hardware/BOM-nixieAccurateClock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Nextcloud\Documents\Projects\nixieclock\nixie-clock-ice\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B659ED1F-74EA-4E36-8957-6581416F1272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7D42A1-4574-4800-A404-6C4D7E983EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="238">
   <si>
     <t>Price</t>
   </si>
@@ -181,9 +181,6 @@
     <t>10u</t>
   </si>
   <si>
-    <t>C12</t>
-  </si>
-  <si>
     <t>SM4004</t>
   </si>
   <si>
@@ -193,18 +190,12 @@
     <t>Conn_Coaxial</t>
   </si>
   <si>
-    <t>Conn_02x05_Odd_Even</t>
-  </si>
-  <si>
     <t>27k</t>
   </si>
   <si>
     <t>100k</t>
   </si>
   <si>
-    <t>R9</t>
-  </si>
-  <si>
     <t>10M</t>
   </si>
   <si>
@@ -496,9 +487,6 @@
     <t>https://www.mouser.com/ProductDetail/CTS-Electronic-Components/219-8MST?qs=qNzHFtQhdJ%252B8jOs%2FDCRqeg%3D%3D</t>
   </si>
   <si>
-    <t>C4, C5, C6, C7, C8, C9, C10, C11</t>
-  </si>
-  <si>
     <t>pico iCE (A)</t>
   </si>
   <si>
@@ -508,42 +496,15 @@
     <t>~</t>
   </si>
   <si>
-    <t>J17</t>
-  </si>
-  <si>
-    <t>L1, L2</t>
-  </si>
-  <si>
     <t>R1, R2</t>
   </si>
   <si>
     <t>R3</t>
   </si>
   <si>
-    <t>R4, R7</t>
-  </si>
-  <si>
-    <t>R5, R8</t>
-  </si>
-  <si>
-    <t>R6</t>
-  </si>
-  <si>
     <t>47k</t>
   </si>
   <si>
-    <t>TP1, TP2, TP3, TP4, TP5, TP6, TP7, TP8, TP9, TP10, TP11, TP12, TP13</t>
-  </si>
-  <si>
-    <t>U4, U5, U6, U7</t>
-  </si>
-  <si>
-    <t>SIB452DK-T1-GE3</t>
-  </si>
-  <si>
-    <t>U10</t>
-  </si>
-  <si>
     <t>UUX2G010MNL1GS</t>
   </si>
   <si>
@@ -556,9 +517,6 @@
     <t>SSM-105-L-DV</t>
   </si>
   <si>
-    <t>M20-7920542R</t>
-  </si>
-  <si>
     <t>SRR1280-100M</t>
   </si>
   <si>
@@ -574,9 +532,6 @@
     <t>:nixie_daughter_board_1</t>
   </si>
   <si>
-    <t>00_lib:SIB452DK-T1-GE3</t>
-  </si>
-  <si>
     <t>00_lib:TXU0104PWR</t>
   </si>
   <si>
@@ -589,18 +544,12 @@
     <t>00_lib:pico iCE (A)</t>
   </si>
   <si>
-    <t>00_lib:M207920542R</t>
-  </si>
-  <si>
     <t>00_lib:IND_BOURNS_SRR1280</t>
   </si>
   <si>
     <t>Potentiometer_SMD:Potentiometer_Bourns_3269X_Horizontal</t>
   </si>
   <si>
-    <t>00_lib:SON_K-T1-GE3_VIS</t>
-  </si>
-  <si>
     <t>Package_SO:TSSOP-14_4.4x5mm_P0.65mm</t>
   </si>
   <si>
@@ -619,9 +568,6 @@
     <t>http://suddendocs.samtec.com/catalog_english/ssm_sm.pdf</t>
   </si>
   <si>
-    <t>https://cdn.harwin.com/pdfs/Harwin_Datasheet-INDESS.pdf</t>
-  </si>
-  <si>
     <t>https://www.bourns.com/docs/Product-Datasheets/SRR1280.pdf</t>
   </si>
   <si>
@@ -649,9 +595,6 @@
     <t>https://www.digikey.com/en/products/detail/samtec-inc/SSM-105-L-DV/1106226</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/harwin-inc/M20-7920542R/6559290</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/bourns-inc/SRR1280-100M/1969992</t>
   </si>
   <si>
@@ -661,9 +604,6 @@
     <t>https://www.digikey.com/en/products/detail/bourns-inc/3269X-1-104GLF/2535630</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/vishay-siliconix/SIB452DK-T1-GE3/1978814</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/texas-instruments/TXU0104PWR/14641439</t>
   </si>
   <si>
@@ -682,9 +622,6 @@
     <t>https://www.mouser.com/ProductDetail/Samtec/SSM-105-L-DV?qs=92ilVni64gwpNieSff7mAQ%3D%3D</t>
   </si>
   <si>
-    <t>https://www.mouser.com/ProductDetail/Harwin/M20-7920542R?qs=k41KVqW3ymqj80AqJ%2FxUlA%3D%3D</t>
-  </si>
-  <si>
     <t>https://www.mouser.com/ProductDetail/Bourns/SRR1280-100M?qs=brMhP%2FMjUfe%2FtbNTKcGHiQ%3D%3D</t>
   </si>
   <si>
@@ -694,28 +631,121 @@
     <t>https://www.mouser.com/ProductDetail/Bourns/3269X-1-104GLF?qs=Rk6YzfsJF02hTa5cSpJqSw%3D%3D</t>
   </si>
   <si>
-    <t>https://www.mouser.com/ProductDetail/Vishay-Semiconductors/SIB452DK-T1-GE3?qs=IRuQNBqMOckO5FjOMoW3mQ%3D%3D</t>
-  </si>
-  <si>
     <t>https://www.mouser.com/ProductDetail/Texas-Instruments/TXU0104PWR?qs=QNEnbhJQKvYcSGbLlthvAQ%3D%3D</t>
   </si>
   <si>
     <t>J4, J5</t>
   </si>
   <si>
-    <t>D1, D2, D3, D4, D5, D6, D7, D8, D9</t>
-  </si>
-  <si>
-    <t>C1, C2, C3, C13, C14, C15, C16, C18, C19, C20, C21</t>
-  </si>
-  <si>
-    <t>J1, J2, J3, J6, J7, J9, J10</t>
-  </si>
-  <si>
-    <t>J11, J12, J13, J14, J15, J16</t>
-  </si>
-  <si>
-    <t>U8, U9, U11, U12</t>
+    <t>C1, C2, C3, C11, C13, C15, C17</t>
+  </si>
+  <si>
+    <t>C4, C5, C6, C7</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>1SMB5956B-13</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>Q1, Q2, Q3, Q4, Q5, Q6</t>
+  </si>
+  <si>
+    <t>PZTA42</t>
+  </si>
+  <si>
+    <t>R4, R11</t>
+  </si>
+  <si>
+    <t>R5, R6, R7, R8</t>
+  </si>
+  <si>
+    <t>R9, R12</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>TP1, TP2, TP3, TP4, TP5, TP6, TP7, TP8, TP9</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>Device:D_Zener</t>
+  </si>
+  <si>
+    <t>:Conn_01x02_Pin_1</t>
+  </si>
+  <si>
+    <t>Transistor_BJT:PZTA42</t>
+  </si>
+  <si>
+    <t>Diode_SMD:D_SMB</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/ds32125.pdf</t>
+  </si>
+  <si>
+    <t>Package_TO_SOT_SMD:SOT-223-3_TabPin2</t>
+  </si>
+  <si>
+    <t>https://www.onsemi.com/pub/Collateral/PZTA42T1-D.PDF</t>
+  </si>
+  <si>
+    <t>Resistor_SMD:R_2010_5025Metric</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/catalog/sei-csr_csrn.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/diodes-incorporated/1SMB5956B-13/5054209</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/micro-commercial-co/PZTA42-TP/10054674</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/CSRN2010FKR500/1742702</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Diodes-Incorporated/1SMB5956B-13?qs=uwKJARvjadOTUcHkJGZGig%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Diotec-Semiconductor/PZTA42?qs=OlC7AqGiEDlNqlN7791aVQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/SEI-Stackpole/CSRN2010FKR500?qs=FESYatJ8odLqZqv0DvLABQ%3D%3D</t>
+  </si>
+  <si>
+    <t>C9, C10, C12, C14, C16</t>
+  </si>
+  <si>
+    <t>D1, D2, D3, D5, D6</t>
+  </si>
+  <si>
+    <t>J1, J2, J3, J9, J10</t>
+  </si>
+  <si>
+    <t>J6, J7</t>
+  </si>
+  <si>
+    <t>J11, J12, J13, J14, J15, J16, J17</t>
+  </si>
+  <si>
+    <t>CSRN2010FKR500</t>
+  </si>
+  <si>
+    <t>U4, U5, U7, U8</t>
   </si>
 </sst>
 </file>
@@ -1083,13 +1113,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA59D120-68A1-4021-9F61-63CF243C8D9C}">
-  <dimension ref="A1:M36"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="89.6640625" customWidth="1"/>
     <col min="4" max="4" width="15.21875" customWidth="1"/>
@@ -1105,7 +1135,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -1113,7 +1143,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>45335.877164351848</v>
+        <v>45345.906342592592</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -1137,7 +1167,8 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>89</v>
+        <f>SUM(B10:B38)</f>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -1180,10 +1211,10 @@
         <v>14</v>
       </c>
       <c r="L9" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="M9" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -1202,7 +1233,7 @@
       <c r="E10">
         <v>3002</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="1">
         <v>0.46</v>
       </c>
       <c r="H10" s="1">
@@ -1210,19 +1241,19 @@
         <v>0.46</v>
       </c>
       <c r="I10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J10" t="s">
+        <v>167</v>
+      </c>
+      <c r="K10" t="s">
+        <v>173</v>
+      </c>
+      <c r="L10" t="s">
         <v>182</v>
       </c>
-      <c r="K10" t="s">
-        <v>190</v>
-      </c>
-      <c r="L10" t="s">
-        <v>200</v>
-      </c>
       <c r="M10" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -1230,10 +1261,10 @@
         <v>2</v>
       </c>
       <c r="B11">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>224</v>
+        <v>201</v>
       </c>
       <c r="D11" t="s">
         <v>18</v>
@@ -1241,15 +1272,15 @@
       <c r="E11" t="s">
         <v>22</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="1">
         <v>0.1</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" ref="H11:H35" si="0">B11*G11</f>
-        <v>1.2000000000000002</v>
+        <f t="shared" ref="H11:H38" si="0">B11*G11</f>
+        <v>0.70000000000000007</v>
       </c>
       <c r="I11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="J11" t="s">
         <v>20</v>
@@ -1258,10 +1289,10 @@
         <v>21</v>
       </c>
       <c r="L11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="M11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -1269,38 +1300,38 @@
         <v>3</v>
       </c>
       <c r="B12">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>154</v>
+        <v>202</v>
       </c>
       <c r="D12" t="s">
         <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>170</v>
-      </c>
-      <c r="G12">
+        <v>157</v>
+      </c>
+      <c r="G12" s="1">
         <v>0.69</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="0"/>
-        <v>5.52</v>
+        <v>2.76</v>
       </c>
       <c r="I12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="J12" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="K12" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
       <c r="L12" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
       <c r="M12" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -1311,15 +1342,15 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>203</v>
       </c>
       <c r="D13" t="s">
         <v>47</v>
       </c>
       <c r="E13" t="s">
-        <v>101</v>
-      </c>
-      <c r="G13">
+        <v>98</v>
+      </c>
+      <c r="G13" s="1">
         <v>0.1</v>
       </c>
       <c r="H13" s="1">
@@ -1327,19 +1358,19 @@
         <v>0.1</v>
       </c>
       <c r="I13" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="J13" t="s">
         <v>20</v>
       </c>
       <c r="K13" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="L13" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="M13" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -1347,38 +1378,38 @@
         <v>5</v>
       </c>
       <c r="B14">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="E14" t="s">
-        <v>50</v>
-      </c>
-      <c r="G14">
-        <v>0.27</v>
+        <v>22</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0.1</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" si="0"/>
-        <v>2.4300000000000002</v>
+        <v>0.5</v>
       </c>
       <c r="I14" t="s">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="J14" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="K14" t="s">
-        <v>78</v>
+        <v>21</v>
       </c>
       <c r="L14" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="M14" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -1386,38 +1417,38 @@
         <v>6</v>
       </c>
       <c r="B15">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="D15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E15" t="s">
-        <v>171</v>
-      </c>
-      <c r="G15">
-        <v>0.42</v>
+        <v>49</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.27</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" si="0"/>
-        <v>2.94</v>
+        <v>1.35</v>
       </c>
       <c r="I15" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="J15" t="s">
-        <v>183</v>
+        <v>74</v>
       </c>
       <c r="K15" t="s">
-        <v>192</v>
+        <v>75</v>
       </c>
       <c r="L15" t="s">
-        <v>202</v>
+        <v>115</v>
       </c>
       <c r="M15" t="s">
-        <v>213</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -1425,38 +1456,35 @@
         <v>7</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>222</v>
+        <v>204</v>
       </c>
       <c r="D16" t="s">
-        <v>155</v>
-      </c>
-      <c r="E16" t="s">
-        <v>172</v>
-      </c>
-      <c r="G16">
-        <v>6.65</v>
+        <v>205</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.46</v>
       </c>
       <c r="H16" s="1">
         <f t="shared" si="0"/>
-        <v>13.3</v>
+        <v>0.46</v>
       </c>
       <c r="I16" t="s">
-        <v>178</v>
+        <v>216</v>
       </c>
       <c r="J16" t="s">
-        <v>184</v>
+        <v>219</v>
       </c>
       <c r="K16" t="s">
-        <v>193</v>
+        <v>220</v>
       </c>
       <c r="L16" t="s">
-        <v>203</v>
+        <v>225</v>
       </c>
       <c r="M16" t="s">
-        <v>214</v>
+        <v>228</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -1464,38 +1492,38 @@
         <v>8</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>156</v>
+        <v>233</v>
       </c>
       <c r="D17" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17">
-        <v>132289</v>
-      </c>
-      <c r="G17">
-        <v>7.55</v>
+        <v>50</v>
+      </c>
+      <c r="E17" t="s">
+        <v>158</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0.42</v>
       </c>
       <c r="H17" s="1">
         <f t="shared" si="0"/>
-        <v>7.55</v>
+        <v>2.1</v>
       </c>
       <c r="I17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="J17" t="s">
-        <v>81</v>
+        <v>168</v>
       </c>
       <c r="K17" t="s">
-        <v>82</v>
+        <v>175</v>
       </c>
       <c r="L17" t="s">
-        <v>121</v>
+        <v>184</v>
       </c>
       <c r="M17" t="s">
-        <v>120</v>
+        <v>193</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
@@ -1503,38 +1531,38 @@
         <v>9</v>
       </c>
       <c r="B18">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>226</v>
+        <v>200</v>
       </c>
       <c r="D18" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="E18" t="s">
-        <v>173</v>
-      </c>
-      <c r="G18">
-        <v>2.59</v>
+        <v>159</v>
+      </c>
+      <c r="G18" s="1">
+        <v>6.65</v>
       </c>
       <c r="H18" s="1">
         <f t="shared" si="0"/>
-        <v>15.54</v>
+        <v>13.3</v>
       </c>
       <c r="I18" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="J18" t="s">
-        <v>97</v>
+        <v>169</v>
       </c>
       <c r="K18" t="s">
+        <v>176</v>
+      </c>
+      <c r="L18" t="s">
+        <v>185</v>
+      </c>
+      <c r="M18" t="s">
         <v>194</v>
-      </c>
-      <c r="L18" t="s">
-        <v>204</v>
-      </c>
-      <c r="M18" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
@@ -1542,38 +1570,38 @@
         <v>10</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C19" t="s">
+        <v>234</v>
+      </c>
+      <c r="D19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" t="s">
         <v>158</v>
       </c>
-      <c r="D19" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" t="s">
-        <v>174</v>
-      </c>
-      <c r="G19">
-        <v>1.71</v>
+      <c r="G19" s="1">
+        <v>0.42</v>
       </c>
       <c r="H19" s="1">
         <f t="shared" si="0"/>
-        <v>1.71</v>
+        <v>0.84</v>
       </c>
       <c r="I19" t="s">
-        <v>24</v>
+        <v>217</v>
       </c>
       <c r="J19" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
       <c r="K19" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="L19" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="M19" t="s">
-        <v>216</v>
+        <v>193</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -1581,38 +1609,38 @@
         <v>11</v>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="D20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" t="s">
-        <v>175</v>
-      </c>
-      <c r="G20">
-        <v>1.02</v>
+        <v>51</v>
+      </c>
+      <c r="E20">
+        <v>132289</v>
+      </c>
+      <c r="G20" s="1">
+        <v>7.55</v>
       </c>
       <c r="H20" s="1">
         <f t="shared" si="0"/>
-        <v>2.04</v>
+        <v>7.55</v>
       </c>
       <c r="I20" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="J20" t="s">
-        <v>186</v>
+        <v>78</v>
       </c>
       <c r="K20" t="s">
-        <v>196</v>
+        <v>79</v>
       </c>
       <c r="L20" t="s">
-        <v>206</v>
+        <v>118</v>
       </c>
       <c r="M20" t="s">
-        <v>217</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
@@ -1620,38 +1648,38 @@
         <v>12</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C21" t="s">
+        <v>235</v>
+      </c>
+      <c r="D21" t="s">
+        <v>153</v>
+      </c>
+      <c r="E21" t="s">
         <v>160</v>
       </c>
-      <c r="D21" t="s">
-        <v>58</v>
-      </c>
-      <c r="E21" t="s">
-        <v>104</v>
-      </c>
-      <c r="G21">
-        <v>0.1</v>
+      <c r="G21" s="1">
+        <v>2.59</v>
       </c>
       <c r="H21" s="1">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>18.13</v>
       </c>
       <c r="I21" t="s">
-        <v>34</v>
+        <v>165</v>
       </c>
       <c r="J21" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="K21" t="s">
-        <v>36</v>
+        <v>177</v>
       </c>
       <c r="L21" t="s">
-        <v>126</v>
+        <v>186</v>
       </c>
       <c r="M21" t="s">
-        <v>127</v>
+        <v>195</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
@@ -1662,35 +1690,35 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
+        <v>206</v>
+      </c>
+      <c r="D22" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" t="s">
         <v>161</v>
       </c>
-      <c r="D22" t="s">
-        <v>57</v>
-      </c>
-      <c r="E22" t="s">
-        <v>103</v>
-      </c>
-      <c r="G22">
-        <v>0.1</v>
+      <c r="G22" s="1">
+        <v>1.02</v>
       </c>
       <c r="H22" s="1">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>1.02</v>
       </c>
       <c r="I22" t="s">
-        <v>34</v>
+        <v>80</v>
       </c>
       <c r="J22" t="s">
-        <v>84</v>
+        <v>170</v>
       </c>
       <c r="K22" t="s">
-        <v>85</v>
+        <v>178</v>
       </c>
       <c r="L22" t="s">
-        <v>124</v>
+        <v>187</v>
       </c>
       <c r="M22" t="s">
-        <v>125</v>
+        <v>196</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
@@ -1698,38 +1726,35 @@
         <v>14</v>
       </c>
       <c r="B23">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>162</v>
+        <v>207</v>
       </c>
       <c r="D23" t="s">
-        <v>55</v>
-      </c>
-      <c r="E23" t="s">
-        <v>102</v>
-      </c>
-      <c r="G23">
-        <v>0.1</v>
+        <v>208</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0.41</v>
       </c>
       <c r="H23" s="1">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>2.46</v>
       </c>
       <c r="I23" t="s">
-        <v>34</v>
+        <v>218</v>
       </c>
       <c r="J23" t="s">
-        <v>84</v>
+        <v>221</v>
       </c>
       <c r="K23" t="s">
-        <v>36</v>
+        <v>222</v>
       </c>
       <c r="L23" t="s">
-        <v>122</v>
+        <v>226</v>
       </c>
       <c r="M23" t="s">
-        <v>123</v>
+        <v>229</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
@@ -1740,15 +1765,15 @@
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="D24" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E24" t="s">
-        <v>105</v>
-      </c>
-      <c r="G24">
+        <v>101</v>
+      </c>
+      <c r="G24" s="1">
         <v>0.1</v>
       </c>
       <c r="H24" s="1">
@@ -1759,16 +1784,16 @@
         <v>34</v>
       </c>
       <c r="J24" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="K24" t="s">
-        <v>85</v>
+        <v>36</v>
       </c>
       <c r="L24" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="M24" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
@@ -1779,35 +1804,35 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="D25" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E25" t="s">
-        <v>136</v>
-      </c>
-      <c r="G25">
-        <v>0.43</v>
+        <v>100</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0.1</v>
       </c>
       <c r="H25" s="1">
         <f t="shared" si="0"/>
-        <v>0.43</v>
+        <v>0.1</v>
       </c>
       <c r="I25" t="s">
         <v>34</v>
       </c>
       <c r="J25" t="s">
-        <v>137</v>
+        <v>81</v>
       </c>
       <c r="K25" t="s">
-        <v>138</v>
+        <v>82</v>
       </c>
       <c r="L25" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="M25" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
@@ -1815,38 +1840,38 @@
         <v>17</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>56</v>
+        <v>209</v>
       </c>
       <c r="D26" t="s">
-        <v>165</v>
+        <v>53</v>
       </c>
       <c r="E26" t="s">
-        <v>176</v>
-      </c>
-      <c r="G26">
+        <v>99</v>
+      </c>
+      <c r="G26" s="1">
         <v>0.1</v>
       </c>
       <c r="H26" s="1">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="I26" t="s">
         <v>34</v>
       </c>
       <c r="J26" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="K26" t="s">
-        <v>197</v>
+        <v>36</v>
       </c>
       <c r="L26" t="s">
-        <v>207</v>
+        <v>119</v>
       </c>
       <c r="M26" t="s">
-        <v>218</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
@@ -1854,38 +1879,38 @@
         <v>18</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>61</v>
-      </c>
-      <c r="D27" t="s">
-        <v>55</v>
+        <v>210</v>
+      </c>
+      <c r="D27">
+        <v>0.5</v>
       </c>
       <c r="E27" t="s">
-        <v>177</v>
-      </c>
-      <c r="G27">
-        <v>3.68</v>
+        <v>236</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0.42</v>
       </c>
       <c r="H27" s="1">
         <f t="shared" si="0"/>
-        <v>3.68</v>
+        <v>1.68</v>
       </c>
       <c r="I27" t="s">
-        <v>86</v>
+        <v>34</v>
       </c>
       <c r="J27" t="s">
-        <v>187</v>
+        <v>223</v>
       </c>
       <c r="K27" t="s">
-        <v>198</v>
+        <v>224</v>
       </c>
       <c r="L27" t="s">
-        <v>208</v>
+        <v>227</v>
       </c>
       <c r="M27" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
@@ -1893,38 +1918,38 @@
         <v>19</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>62</v>
+        <v>211</v>
       </c>
       <c r="D28" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E28" t="s">
-        <v>149</v>
-      </c>
-      <c r="G28">
-        <v>0.95</v>
+        <v>102</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0.1</v>
       </c>
       <c r="H28" s="1">
         <f t="shared" si="0"/>
-        <v>0.95</v>
+        <v>0.2</v>
       </c>
       <c r="I28" t="s">
-        <v>87</v>
+        <v>34</v>
       </c>
       <c r="J28" t="s">
-        <v>150</v>
+        <v>81</v>
       </c>
       <c r="K28" t="s">
-        <v>151</v>
+        <v>82</v>
       </c>
       <c r="L28" t="s">
-        <v>152</v>
+        <v>126</v>
       </c>
       <c r="M28" t="s">
-        <v>153</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
@@ -1932,38 +1957,38 @@
         <v>20</v>
       </c>
       <c r="B29">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>166</v>
+        <v>212</v>
       </c>
       <c r="D29" t="s">
-        <v>64</v>
-      </c>
-      <c r="E29">
-        <v>5019</v>
-      </c>
-      <c r="G29">
-        <v>0.33</v>
+        <v>56</v>
+      </c>
+      <c r="E29" t="s">
+        <v>133</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0.43</v>
       </c>
       <c r="H29" s="1">
         <f t="shared" si="0"/>
-        <v>4.29</v>
+        <v>0.43</v>
       </c>
       <c r="I29" t="s">
-        <v>88</v>
+        <v>34</v>
       </c>
       <c r="J29" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="K29" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="L29" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="M29" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
@@ -1974,32 +1999,35 @@
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>37</v>
+        <v>213</v>
       </c>
       <c r="D30" t="s">
-        <v>65</v>
-      </c>
-      <c r="G30">
-        <v>1.37</v>
+        <v>156</v>
+      </c>
+      <c r="E30" t="s">
+        <v>162</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0.1</v>
       </c>
       <c r="H30" s="1">
         <f t="shared" si="0"/>
-        <v>1.37</v>
+        <v>0.1</v>
       </c>
       <c r="I30" t="s">
-        <v>89</v>
+        <v>34</v>
       </c>
       <c r="J30" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="K30" t="s">
-        <v>91</v>
+        <v>179</v>
       </c>
       <c r="L30" t="s">
-        <v>131</v>
+        <v>188</v>
       </c>
       <c r="M30" t="s">
-        <v>130</v>
+        <v>197</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
@@ -2010,32 +2038,35 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D31" t="s">
-        <v>68</v>
-      </c>
-      <c r="G31">
-        <v>0.97</v>
+        <v>53</v>
+      </c>
+      <c r="E31" t="s">
+        <v>163</v>
+      </c>
+      <c r="G31" s="1">
+        <v>3.68</v>
       </c>
       <c r="H31" s="1">
         <f t="shared" si="0"/>
-        <v>0.97</v>
+        <v>3.68</v>
       </c>
       <c r="I31" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="J31" t="s">
-        <v>93</v>
+        <v>171</v>
       </c>
       <c r="K31" t="s">
-        <v>94</v>
+        <v>180</v>
       </c>
       <c r="L31" t="s">
-        <v>132</v>
+        <v>189</v>
       </c>
       <c r="M31" t="s">
-        <v>133</v>
+        <v>198</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
@@ -2046,32 +2077,35 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D32" t="s">
-        <v>69</v>
-      </c>
-      <c r="G32">
-        <v>27.8</v>
+        <v>60</v>
+      </c>
+      <c r="E32" t="s">
+        <v>146</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0.95</v>
       </c>
       <c r="H32" s="1">
         <f t="shared" si="0"/>
-        <v>27.8</v>
+        <v>0.95</v>
       </c>
       <c r="I32" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="J32" t="s">
-        <v>95</v>
+        <v>147</v>
       </c>
       <c r="K32" t="s">
-        <v>96</v>
+        <v>148</v>
       </c>
       <c r="L32" t="s">
-        <v>113</v>
+        <v>149</v>
       </c>
       <c r="M32" t="s">
-        <v>113</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
@@ -2079,35 +2113,38 @@
         <v>24</v>
       </c>
       <c r="B33">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C33" t="s">
-        <v>167</v>
+        <v>214</v>
       </c>
       <c r="D33" t="s">
-        <v>168</v>
-      </c>
-      <c r="G33">
-        <v>0.76</v>
+        <v>61</v>
+      </c>
+      <c r="E33">
+        <v>5019</v>
+      </c>
+      <c r="G33" s="1">
+        <v>0.33</v>
       </c>
       <c r="H33" s="1">
         <f t="shared" si="0"/>
-        <v>3.04</v>
+        <v>2.97</v>
       </c>
       <c r="I33" t="s">
-        <v>180</v>
+        <v>85</v>
       </c>
       <c r="J33" t="s">
-        <v>188</v>
+        <v>141</v>
       </c>
       <c r="K33" t="s">
-        <v>168</v>
+        <v>140</v>
       </c>
       <c r="L33" t="s">
-        <v>209</v>
+        <v>138</v>
       </c>
       <c r="M33" t="s">
-        <v>220</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
@@ -2115,35 +2152,35 @@
         <v>25</v>
       </c>
       <c r="B34">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>227</v>
+        <v>37</v>
       </c>
       <c r="D34" t="s">
-        <v>157</v>
-      </c>
-      <c r="G34">
-        <v>0.83</v>
+        <v>62</v>
+      </c>
+      <c r="G34" s="1">
+        <v>1.37</v>
       </c>
       <c r="H34" s="1">
         <f t="shared" si="0"/>
-        <v>3.32</v>
+        <v>1.37</v>
       </c>
       <c r="I34" t="s">
-        <v>181</v>
+        <v>86</v>
       </c>
       <c r="J34" t="s">
-        <v>189</v>
+        <v>87</v>
       </c>
       <c r="K34" t="s">
-        <v>199</v>
+        <v>88</v>
       </c>
       <c r="L34" t="s">
-        <v>210</v>
+        <v>128</v>
       </c>
       <c r="M34" t="s">
-        <v>221</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
@@ -2154,41 +2191,149 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>169</v>
+        <v>63</v>
       </c>
       <c r="D35" t="s">
-        <v>70</v>
-      </c>
-      <c r="E35" t="s">
-        <v>106</v>
-      </c>
-      <c r="G35">
-        <v>5.93</v>
+        <v>65</v>
+      </c>
+      <c r="G35" s="1">
+        <v>0.97</v>
       </c>
       <c r="H35" s="1">
         <f t="shared" si="0"/>
+        <v>0.97</v>
+      </c>
+      <c r="I35" t="s">
+        <v>89</v>
+      </c>
+      <c r="J35" t="s">
+        <v>90</v>
+      </c>
+      <c r="K35" t="s">
+        <v>91</v>
+      </c>
+      <c r="L35" t="s">
+        <v>129</v>
+      </c>
+      <c r="M35" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>27</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" t="s">
+        <v>66</v>
+      </c>
+      <c r="G36" s="1">
+        <v>27.8</v>
+      </c>
+      <c r="H36" s="1">
+        <f t="shared" si="0"/>
+        <v>27.8</v>
+      </c>
+      <c r="I36" t="s">
+        <v>92</v>
+      </c>
+      <c r="J36" t="s">
+        <v>92</v>
+      </c>
+      <c r="K36" t="s">
+        <v>93</v>
+      </c>
+      <c r="L36" t="s">
+        <v>110</v>
+      </c>
+      <c r="M36" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>28</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>237</v>
+      </c>
+      <c r="D37" t="s">
+        <v>153</v>
+      </c>
+      <c r="G37" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="H37" s="1">
+        <f t="shared" si="0"/>
+        <v>3.32</v>
+      </c>
+      <c r="I37" t="s">
+        <v>166</v>
+      </c>
+      <c r="J37" t="s">
+        <v>172</v>
+      </c>
+      <c r="K37" t="s">
+        <v>181</v>
+      </c>
+      <c r="L37" t="s">
+        <v>190</v>
+      </c>
+      <c r="M37" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>29</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>215</v>
+      </c>
+      <c r="D38" t="s">
+        <v>67</v>
+      </c>
+      <c r="E38" t="s">
+        <v>103</v>
+      </c>
+      <c r="G38" s="1">
         <v>5.93</v>
       </c>
-      <c r="I35" t="s">
-        <v>98</v>
-      </c>
-      <c r="J35" t="s">
-        <v>99</v>
-      </c>
-      <c r="K35" t="s">
-        <v>100</v>
-      </c>
-      <c r="L35" t="s">
-        <v>134</v>
-      </c>
-      <c r="M35" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="G36">
-        <f>SUM(G10:G35)</f>
-        <v>65.11</v>
+      <c r="H38" s="1">
+        <f t="shared" si="0"/>
+        <v>5.93</v>
+      </c>
+      <c r="I38" t="s">
+        <v>95</v>
+      </c>
+      <c r="J38" t="s">
+        <v>96</v>
+      </c>
+      <c r="K38" t="s">
+        <v>97</v>
+      </c>
+      <c r="L38" t="s">
+        <v>131</v>
+      </c>
+      <c r="M38" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="H39" s="1">
+        <f>SUM(H10:H38)</f>
+        <v>101.63</v>
       </c>
     </row>
   </sheetData>
@@ -2293,10 +2438,10 @@
         <v>14</v>
       </c>
       <c r="L9" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="M9" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -2332,10 +2477,10 @@
         <v>21</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -2368,10 +2513,10 @@
         <v>26</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="M11" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -2404,10 +2549,10 @@
         <v>32</v>
       </c>
       <c r="L12" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="M12" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -2421,10 +2566,10 @@
         <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E13" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G13" s="1">
         <v>0.1</v>
@@ -2443,10 +2588,10 @@
         <v>36</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -2479,10 +2624,10 @@
         <v>41</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>